<commit_message>
update test ứng dụng
</commit_message>
<xml_diff>
--- a/test_ung_dung.xlsx
+++ b/test_ung_dung.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="197">
   <si>
     <t>STT</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Check khách hàng với ID: NV032 (thêm từ hồi test QLKhachHang.xaml)</t>
   </si>
   <si>
-    <t>Fail vì khách hàng chỉ mã ID là KH</t>
-  </si>
-  <si>
     <t>Lập hóa đơn khách hàng với ID: KH001</t>
   </si>
   <si>
@@ -384,9 +381,6 @@
     <t>thông báo sai mã hóa đơn</t>
   </si>
   <si>
-    <t>fail</t>
-  </si>
-  <si>
     <t>lập HD mới, dán ID hóa đơn cũ vào, thêm sản phẩm vào</t>
   </si>
   <si>
@@ -436,9 +430,6 @@
   </si>
   <si>
     <t xml:space="preserve">chưa khóa </t>
-  </si>
-  <si>
-    <t>fail (không sai về chức năng, nhưng sai hình thức)</t>
   </si>
   <si>
     <t>search hóa đơn đã có</t>
@@ -652,7 +643,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -684,6 +675,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2EF24F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -771,7 +768,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -812,6 +809,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -819,15 +822,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -848,25 +842,48 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Chuẩn" xfId="0" builtinId="0"/>
+    <cellStyle name="Tốt" xfId="1" builtinId="26"/>
+    <cellStyle name="Xấu" xfId="2" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF2EF24F"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -883,7 +900,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2720340</xdr:colOff>
+      <xdr:colOff>2682240</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>52256</xdr:rowOff>
     </xdr:to>
@@ -926,8 +943,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2746288</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3088</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>6515</xdr:rowOff>
     </xdr:to>
@@ -1014,8 +1031,8 @@
       <xdr:rowOff>53724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2727960</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>99525</xdr:rowOff>
     </xdr:to>
@@ -1103,7 +1120,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2759825</xdr:colOff>
+      <xdr:colOff>2683625</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>91439</xdr:rowOff>
     </xdr:to>
@@ -1190,8 +1207,8 @@
       <xdr:rowOff>46196</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2659380</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>87629</xdr:rowOff>
     </xdr:to>
@@ -1278,8 +1295,8 @@
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2727517</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3367</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>68782</xdr:rowOff>
     </xdr:to>
@@ -1454,8 +1471,8 @@
       <xdr:rowOff>12105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2689859</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3809</xdr:colOff>
       <xdr:row>130</xdr:row>
       <xdr:rowOff>22197</xdr:rowOff>
     </xdr:to>
@@ -1499,7 +1516,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2758441</xdr:colOff>
+      <xdr:colOff>2682241</xdr:colOff>
       <xdr:row>140</xdr:row>
       <xdr:rowOff>99794</xdr:rowOff>
     </xdr:to>
@@ -1542,8 +1559,8 @@
       <xdr:rowOff>51354</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2735580</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
       <xdr:row>153</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
@@ -1586,8 +1603,8 @@
       <xdr:rowOff>40957</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2613659</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3809</xdr:colOff>
       <xdr:row>153</xdr:row>
       <xdr:rowOff>26669</xdr:rowOff>
     </xdr:to>
@@ -1630,8 +1647,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2735578</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1903</xdr:colOff>
       <xdr:row>171</xdr:row>
       <xdr:rowOff>43245</xdr:rowOff>
     </xdr:to>
@@ -1675,7 +1692,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2644140</xdr:colOff>
+      <xdr:colOff>2606040</xdr:colOff>
       <xdr:row>184</xdr:row>
       <xdr:rowOff>26668</xdr:rowOff>
     </xdr:to>
@@ -1718,8 +1735,8 @@
       <xdr:rowOff>71436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2621280</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
       <xdr:row>197</xdr:row>
       <xdr:rowOff>57148</xdr:rowOff>
     </xdr:to>
@@ -1800,7 +1817,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1835,7 +1852,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2046,23 +2063,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="F162" sqref="F162:F163"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="F232" sqref="F232"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="27.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2085,7 +2102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2098,597 +2115,597 @@
       <c r="F2" s="8"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23">
+    <row r="3" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="23" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="21"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="21"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="20"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="21"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="20"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="21"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="20"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="21"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="22"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23">
+    <row r="11" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22">
         <v>1.2</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="23" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="23" t="s">
+      <c r="D11" s="16"/>
+      <c r="E11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="21"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="21"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="21"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="21"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="21"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="21"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="21"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="22"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="21"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23">
+    <row r="20" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22">
         <v>1.3</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="23" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="23" t="s">
+      <c r="D20" s="16"/>
+      <c r="E20" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="21"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="21"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="21"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="21"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="21"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="23"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="21"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="21"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="20"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="23"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="22"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23">
+    <row r="29" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
         <v>1.4</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="23" t="s">
+      <c r="B29" s="17"/>
+      <c r="C29" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="23" t="s">
+      <c r="D29" s="16"/>
+      <c r="E29" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="23"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="21"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="20"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="23"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="21"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="21"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="23"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="21"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="23"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="21"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="20"/>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="21"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="20"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="23"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="21"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="20"/>
       <c r="G36" s="10"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="21"/>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="20"/>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="23"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="22"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="22"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="21"/>
       <c r="G38" s="10"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="23">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="22">
         <v>1.5</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="C39" s="23" t="s">
+      <c r="B39" s="17"/>
+      <c r="C39" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="14"/>
+      <c r="D39" s="16"/>
       <c r="E39" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="15"/>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="22"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="17"/>
       <c r="E40" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F40" s="21"/>
+      <c r="F40" s="20"/>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="23"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="14" t="s">
+    <row r="41" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="22"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F41" s="21"/>
+      <c r="F41" s="20"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="21"/>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="22"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="20"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="21"/>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="20"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="21"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="20"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="23"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="21"/>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="22"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="20"/>
       <c r="G45" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="23"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="21"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="22"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="20"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="21"/>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="22"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="20"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="23"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="21"/>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="22"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="20"/>
       <c r="G48" s="10"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="23"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="21"/>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="22"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="20"/>
       <c r="G49" s="10"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="23"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="22"/>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="22"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="21"/>
       <c r="G50" s="10"/>
     </row>
-    <row r="51" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>1.6</v>
       </c>
-      <c r="B51" s="15"/>
-      <c r="C51" s="23" t="s">
+      <c r="B51" s="17"/>
+      <c r="C51" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="23" t="s">
+      <c r="D51" s="16"/>
+      <c r="E51" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F51" s="20" t="s">
+      <c r="F51" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G51" s="10"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="21"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="20"/>
       <c r="G52" s="10"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="21"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="20"/>
       <c r="G53" s="10"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="21"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="20"/>
       <c r="G54" s="10"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="21"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="20"/>
       <c r="G55" s="10"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="21"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="20"/>
       <c r="G56" s="10"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="21"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="20"/>
       <c r="G57" s="10"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="21"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="20"/>
       <c r="G58" s="10"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="21"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="20"/>
       <c r="G59" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
-      <c r="B60" s="15"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="23"/>
-      <c r="F60" s="22"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="21"/>
       <c r="G60" s="10"/>
     </row>
-    <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
         <v>1.7</v>
       </c>
-      <c r="B61" s="15"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="10" t="s">
         <v>23</v>
       </c>
@@ -2701,11 +2718,11 @@
       </c>
       <c r="G61" s="10"/>
     </row>
-    <row r="62" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
         <v>1.8</v>
       </c>
-      <c r="B62" s="15"/>
+      <c r="B62" s="17"/>
       <c r="C62" s="10" t="s">
         <v>25</v>
       </c>
@@ -2718,11 +2735,11 @@
       </c>
       <c r="G62" s="10"/>
     </row>
-    <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>1.9</v>
       </c>
-      <c r="B63" s="15"/>
+      <c r="B63" s="17"/>
       <c r="C63" s="10" t="s">
         <v>26</v>
       </c>
@@ -2735,11 +2752,11 @@
       </c>
       <c r="G63" s="10"/>
     </row>
-    <row r="64" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="15"/>
+      <c r="B64" s="17"/>
       <c r="C64" s="10" t="s">
         <v>28</v>
       </c>
@@ -2752,11 +2769,11 @@
       </c>
       <c r="G64" s="10"/>
     </row>
-    <row r="65" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B65" s="15"/>
+      <c r="B65" s="17"/>
       <c r="C65" s="10" t="s">
         <v>30</v>
       </c>
@@ -2769,11 +2786,11 @@
       </c>
       <c r="G65" s="10"/>
     </row>
-    <row r="66" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B66" s="15"/>
+      <c r="B66" s="17"/>
       <c r="C66" s="10" t="s">
         <v>32</v>
       </c>
@@ -2786,11 +2803,11 @@
       </c>
       <c r="G66" s="10"/>
     </row>
-    <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B67" s="15"/>
+      <c r="B67" s="17"/>
       <c r="C67" s="10" t="s">
         <v>33</v>
       </c>
@@ -2802,338 +2819,338 @@
         <v>10</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B68" s="15"/>
-      <c r="C68" s="23" t="s">
+      <c r="B68" s="17"/>
+      <c r="C68" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D68" s="14"/>
-      <c r="E68" s="23" t="s">
+      <c r="D68" s="16"/>
+      <c r="E68" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F68" s="25" t="s">
+      <c r="F68" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G68" s="10"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="23"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="23"/>
-      <c r="F69" s="25"/>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="22"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="24"/>
       <c r="G69" s="10"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="23"/>
-      <c r="B70" s="15"/>
-      <c r="C70" s="23"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="23"/>
-      <c r="F70" s="25"/>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="22"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="24"/>
       <c r="G70" s="10"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="23"/>
-      <c r="B71" s="15"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="25"/>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="22"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="24"/>
       <c r="G71" s="10"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="23"/>
-      <c r="B72" s="15"/>
-      <c r="C72" s="23"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="25"/>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="22"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="24"/>
       <c r="G72" s="10"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="23"/>
-      <c r="B73" s="15"/>
-      <c r="C73" s="23"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="25"/>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="22"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="24"/>
       <c r="G73" s="10"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="23"/>
-      <c r="B74" s="15"/>
-      <c r="C74" s="23"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="25"/>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="22"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="24"/>
       <c r="G74" s="10"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="23"/>
-      <c r="B75" s="15"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="25"/>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="22"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="24"/>
       <c r="G75" s="10"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="23"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="23"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="23"/>
-      <c r="F76" s="25"/>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="22"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="24"/>
       <c r="G76" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="23"/>
-      <c r="B77" s="15"/>
-      <c r="C77" s="23"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="23"/>
-      <c r="F77" s="25"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="22"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="24"/>
       <c r="G77" s="10"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="23"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="23"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="23"/>
-      <c r="F78" s="25"/>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="22"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="24"/>
       <c r="G78" s="10"/>
     </row>
-    <row r="79" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="14" t="s">
+    <row r="79" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B79" s="15"/>
-      <c r="C79" s="14" t="s">
+      <c r="B79" s="17"/>
+      <c r="C79" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D79" s="14"/>
-      <c r="E79" s="23" t="s">
+      <c r="D79" s="16"/>
+      <c r="E79" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F79" s="24" t="s">
+      <c r="F79" s="23" t="s">
         <v>39</v>
       </c>
       <c r="G79" s="10"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="15"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="23"/>
-      <c r="F80" s="24"/>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="17"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="23"/>
       <c r="G80" s="10"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="15"/>
-      <c r="B81" s="15"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="23"/>
-      <c r="F81" s="24"/>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="17"/>
+      <c r="B81" s="17"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="23"/>
       <c r="G81" s="10"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="15"/>
-      <c r="B82" s="15"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="23"/>
-      <c r="F82" s="24"/>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="17"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="23"/>
       <c r="G82" s="10"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="15"/>
-      <c r="B83" s="15"/>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
-      <c r="E83" s="23"/>
-      <c r="F83" s="24"/>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="17"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="23"/>
       <c r="G83" s="10"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" s="15"/>
-      <c r="B84" s="15"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="15"/>
-      <c r="E84" s="23"/>
-      <c r="F84" s="24"/>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="17"/>
+      <c r="B84" s="17"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="23"/>
       <c r="G84" s="10"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="15"/>
-      <c r="B85" s="15"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
-      <c r="E85" s="23"/>
-      <c r="F85" s="24"/>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="17"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="23"/>
       <c r="G85" s="10"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="15"/>
-      <c r="B86" s="15"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="23"/>
-      <c r="F86" s="24"/>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="17"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="23"/>
       <c r="G86" s="10"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="15"/>
-      <c r="B87" s="15"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="23"/>
-      <c r="F87" s="24"/>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="17"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="23"/>
       <c r="G87" s="10"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="15"/>
-      <c r="B88" s="15"/>
-      <c r="C88" s="15"/>
-      <c r="D88" s="15"/>
-      <c r="E88" s="23"/>
-      <c r="F88" s="24"/>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="17"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="23"/>
       <c r="G88" s="10"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="16"/>
-      <c r="B89" s="16"/>
-      <c r="C89" s="16"/>
-      <c r="D89" s="16"/>
-      <c r="E89" s="23"/>
-      <c r="F89" s="24"/>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="18"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="22"/>
+      <c r="F89" s="23"/>
       <c r="G89" s="10"/>
     </row>
-    <row r="90" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
         <v>1.1599999999999999</v>
       </c>
       <c r="B90" s="11"/>
       <c r="C90" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D90" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D90" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E90" s="26" t="s">
-        <v>113</v>
+      <c r="E90" s="14" t="s">
+        <v>112</v>
       </c>
       <c r="F90" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G90" s="10"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="11">
         <v>1.17</v>
       </c>
       <c r="B91" s="11"/>
       <c r="C91" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D91" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D91" s="11" t="s">
+      <c r="E91" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E91" s="26" t="s">
-        <v>107</v>
-      </c>
       <c r="F91" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G91" s="10"/>
     </row>
-    <row r="92" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="11">
         <v>1.18</v>
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D92" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D92" s="11" t="s">
+      <c r="E92" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E92" s="26" t="s">
-        <v>110</v>
-      </c>
       <c r="F92" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G92" s="10"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="11">
         <v>1.19</v>
       </c>
       <c r="B93" s="11"/>
       <c r="C93" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D93" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D93" s="11" t="s">
+      <c r="E93" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="E93" s="26" t="s">
-        <v>113</v>
-      </c>
       <c r="F93" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G93" s="10"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B94" s="11"/>
       <c r="C94" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D94" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D94" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E94" s="26"/>
+      <c r="E94" s="14"/>
       <c r="F94" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G94" s="10"/>
     </row>
-    <row r="95" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="11">
         <v>1.21</v>
       </c>
       <c r="B95" s="11"/>
       <c r="C95" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E95" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="D95" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="E95" s="26" t="s">
-        <v>191</v>
-      </c>
       <c r="F95" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G95" s="10"/>
     </row>
-    <row r="96" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>2</v>
       </c>
@@ -3146,150 +3163,150 @@
       <c r="F96" s="9"/>
       <c r="G96" s="9"/>
     </row>
-    <row r="97" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="14">
+    <row r="97" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="16">
         <v>2.1</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C97" s="14" t="s">
+      <c r="C97" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D97" s="14"/>
-      <c r="E97" s="14" t="s">
+      <c r="D97" s="16"/>
+      <c r="E97" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F97" s="17" t="s">
+      <c r="F97" s="25" t="s">
         <v>45</v>
       </c>
       <c r="G97" s="10"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" s="15"/>
-      <c r="B98" s="15"/>
-      <c r="C98" s="15"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="15"/>
-      <c r="F98" s="18"/>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="17"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="26"/>
       <c r="G98" s="10"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="15"/>
-      <c r="B99" s="15"/>
-      <c r="C99" s="15"/>
-      <c r="D99" s="15"/>
-      <c r="E99" s="15"/>
-      <c r="F99" s="18"/>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="17"/>
+      <c r="B99" s="17"/>
+      <c r="C99" s="17"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="26"/>
       <c r="G99" s="10"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="15"/>
-      <c r="B100" s="15"/>
-      <c r="C100" s="15"/>
-      <c r="D100" s="15"/>
-      <c r="E100" s="15"/>
-      <c r="F100" s="18"/>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="17"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="26"/>
       <c r="G100" s="10"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" s="15"/>
-      <c r="B101" s="15"/>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
-      <c r="E101" s="15"/>
-      <c r="F101" s="18"/>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="17"/>
+      <c r="B101" s="17"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="26"/>
       <c r="G101" s="10"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="15"/>
-      <c r="B102" s="15"/>
-      <c r="C102" s="15"/>
-      <c r="D102" s="15"/>
-      <c r="E102" s="15"/>
-      <c r="F102" s="18"/>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="17"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="26"/>
       <c r="G102" s="10"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A103" s="15"/>
-      <c r="B103" s="15"/>
-      <c r="C103" s="15"/>
-      <c r="D103" s="15"/>
-      <c r="E103" s="15"/>
-      <c r="F103" s="18"/>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="17"/>
+      <c r="B103" s="17"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="26"/>
       <c r="G103" s="10"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" s="15"/>
-      <c r="B104" s="15"/>
-      <c r="C104" s="15"/>
-      <c r="D104" s="15"/>
-      <c r="E104" s="15"/>
-      <c r="F104" s="18"/>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="17"/>
+      <c r="B104" s="17"/>
+      <c r="C104" s="17"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="17"/>
+      <c r="F104" s="26"/>
       <c r="G104" s="10"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A105" s="15"/>
-      <c r="B105" s="15"/>
-      <c r="C105" s="15"/>
-      <c r="D105" s="15"/>
-      <c r="E105" s="15"/>
-      <c r="F105" s="18"/>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="17"/>
+      <c r="B105" s="17"/>
+      <c r="C105" s="17"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="26"/>
       <c r="G105" s="10"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="16"/>
-      <c r="B106" s="15"/>
-      <c r="C106" s="16"/>
-      <c r="D106" s="16"/>
-      <c r="E106" s="16"/>
-      <c r="F106" s="19"/>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="18"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="27"/>
       <c r="G106" s="10"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="14">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="16">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B107" s="15"/>
-      <c r="C107" s="14" t="s">
+      <c r="B107" s="17"/>
+      <c r="C107" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D107" s="14"/>
+      <c r="D107" s="16"/>
       <c r="E107" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F107" s="17" t="s">
+      <c r="F107" s="25" t="s">
         <v>16</v>
       </c>
       <c r="G107" s="10"/>
     </row>
-    <row r="108" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A108" s="15"/>
-      <c r="B108" s="15"/>
-      <c r="C108" s="15"/>
-      <c r="D108" s="15"/>
+    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="17"/>
+      <c r="B108" s="17"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="17"/>
       <c r="E108" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F108" s="18"/>
+      <c r="F108" s="26"/>
       <c r="G108" s="10"/>
     </row>
-    <row r="109" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A109" s="16"/>
-      <c r="B109" s="15"/>
-      <c r="C109" s="16"/>
-      <c r="D109" s="16"/>
+    <row r="109" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A109" s="18"/>
+      <c r="B109" s="17"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18"/>
       <c r="E109" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F109" s="19"/>
+      <c r="F109" s="27"/>
       <c r="G109" s="10"/>
     </row>
-    <row r="110" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="10">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B110" s="15"/>
+      <c r="B110" s="17"/>
       <c r="C110" s="10" t="s">
         <v>46</v>
       </c>
@@ -3302,11 +3319,11 @@
       </c>
       <c r="G110" s="10"/>
     </row>
-    <row r="111" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="10">
         <v>2.4</v>
       </c>
-      <c r="B111" s="15"/>
+      <c r="B111" s="17"/>
       <c r="C111" s="10" t="s">
         <v>50</v>
       </c>
@@ -3319,11 +3336,11 @@
       </c>
       <c r="G111" s="10"/>
     </row>
-    <row r="112" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="10">
         <v>2.5</v>
       </c>
-      <c r="B112" s="15"/>
+      <c r="B112" s="17"/>
       <c r="C112" s="10" t="s">
         <v>52</v>
       </c>
@@ -3336,323 +3353,323 @@
       </c>
       <c r="G112" s="10"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A113" s="14">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="16">
         <v>2.6</v>
       </c>
-      <c r="B113" s="15"/>
-      <c r="C113" s="14" t="s">
+      <c r="B113" s="17"/>
+      <c r="C113" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14" t="s">
+      <c r="D113" s="16"/>
+      <c r="E113" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F113" s="20" t="s">
+      <c r="F113" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G113" s="10"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A114" s="15"/>
-      <c r="B114" s="15"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="15"/>
-      <c r="E114" s="15"/>
-      <c r="F114" s="21"/>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="17"/>
+      <c r="B114" s="17"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="17"/>
+      <c r="F114" s="20"/>
       <c r="G114" s="10"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A115" s="15"/>
-      <c r="B115" s="15"/>
-      <c r="C115" s="15"/>
-      <c r="D115" s="15"/>
-      <c r="E115" s="15"/>
-      <c r="F115" s="21"/>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="17"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="17"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="17"/>
+      <c r="F115" s="20"/>
       <c r="G115" s="10"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A116" s="15"/>
-      <c r="B116" s="15"/>
-      <c r="C116" s="15"/>
-      <c r="D116" s="15"/>
-      <c r="E116" s="15"/>
-      <c r="F116" s="21"/>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="17"/>
+      <c r="B116" s="17"/>
+      <c r="C116" s="17"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="17"/>
+      <c r="F116" s="20"/>
       <c r="G116" s="10"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="15"/>
-      <c r="B117" s="15"/>
-      <c r="C117" s="15"/>
-      <c r="D117" s="15"/>
-      <c r="E117" s="15"/>
-      <c r="F117" s="21"/>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="17"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="17"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="17"/>
+      <c r="F117" s="20"/>
       <c r="G117" s="10"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A118" s="15"/>
-      <c r="B118" s="15"/>
-      <c r="C118" s="15"/>
-      <c r="D118" s="15"/>
-      <c r="E118" s="15"/>
-      <c r="F118" s="21"/>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="17"/>
+      <c r="B118" s="17"/>
+      <c r="C118" s="17"/>
+      <c r="D118" s="17"/>
+      <c r="E118" s="17"/>
+      <c r="F118" s="20"/>
       <c r="G118" s="10"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A119" s="15"/>
-      <c r="B119" s="15"/>
-      <c r="C119" s="15"/>
-      <c r="D119" s="15"/>
-      <c r="E119" s="15"/>
-      <c r="F119" s="21"/>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="17"/>
+      <c r="B119" s="17"/>
+      <c r="C119" s="17"/>
+      <c r="D119" s="17"/>
+      <c r="E119" s="17"/>
+      <c r="F119" s="20"/>
       <c r="G119" s="10"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A120" s="15"/>
-      <c r="B120" s="15"/>
-      <c r="C120" s="15"/>
-      <c r="D120" s="15"/>
-      <c r="E120" s="15"/>
-      <c r="F120" s="21"/>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="17"/>
+      <c r="B120" s="17"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="20"/>
       <c r="G120" s="10"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A121" s="15"/>
-      <c r="B121" s="15"/>
-      <c r="C121" s="15"/>
-      <c r="D121" s="15"/>
-      <c r="E121" s="15"/>
-      <c r="F121" s="21"/>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="17"/>
+      <c r="B121" s="17"/>
+      <c r="C121" s="17"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="20"/>
       <c r="G121" s="10"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A122" s="16"/>
-      <c r="B122" s="15"/>
-      <c r="C122" s="16"/>
-      <c r="D122" s="16"/>
-      <c r="E122" s="16"/>
-      <c r="F122" s="22"/>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="18"/>
+      <c r="B122" s="17"/>
+      <c r="C122" s="18"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="18"/>
+      <c r="F122" s="21"/>
       <c r="G122" s="10"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A123" s="14">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="16">
         <v>2.7</v>
       </c>
-      <c r="B123" s="15"/>
-      <c r="C123" s="14" t="s">
+      <c r="B123" s="17"/>
+      <c r="C123" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D123" s="14"/>
-      <c r="E123" s="14" t="s">
+      <c r="D123" s="16"/>
+      <c r="E123" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F123" s="20" t="s">
+      <c r="F123" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G123" s="10"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A124" s="15"/>
-      <c r="B124" s="15"/>
-      <c r="C124" s="15"/>
-      <c r="D124" s="15"/>
-      <c r="E124" s="15"/>
-      <c r="F124" s="21"/>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="17"/>
+      <c r="B124" s="17"/>
+      <c r="C124" s="17"/>
+      <c r="D124" s="17"/>
+      <c r="E124" s="17"/>
+      <c r="F124" s="20"/>
       <c r="G124" s="10"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A125" s="15"/>
-      <c r="B125" s="15"/>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
-      <c r="E125" s="15"/>
-      <c r="F125" s="21"/>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="17"/>
+      <c r="B125" s="17"/>
+      <c r="C125" s="17"/>
+      <c r="D125" s="17"/>
+      <c r="E125" s="17"/>
+      <c r="F125" s="20"/>
       <c r="G125" s="10"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A126" s="15"/>
-      <c r="B126" s="15"/>
-      <c r="C126" s="15"/>
-      <c r="D126" s="15"/>
-      <c r="E126" s="15"/>
-      <c r="F126" s="21"/>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="17"/>
+      <c r="B126" s="17"/>
+      <c r="C126" s="17"/>
+      <c r="D126" s="17"/>
+      <c r="E126" s="17"/>
+      <c r="F126" s="20"/>
       <c r="G126" s="10"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" s="15"/>
-      <c r="B127" s="15"/>
-      <c r="C127" s="15"/>
-      <c r="D127" s="15"/>
-      <c r="E127" s="15"/>
-      <c r="F127" s="21"/>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="17"/>
+      <c r="B127" s="17"/>
+      <c r="C127" s="17"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="17"/>
+      <c r="F127" s="20"/>
       <c r="G127" s="10"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A128" s="15"/>
-      <c r="B128" s="15"/>
-      <c r="C128" s="15"/>
-      <c r="D128" s="15"/>
-      <c r="E128" s="15"/>
-      <c r="F128" s="21"/>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="17"/>
+      <c r="B128" s="17"/>
+      <c r="C128" s="17"/>
+      <c r="D128" s="17"/>
+      <c r="E128" s="17"/>
+      <c r="F128" s="20"/>
       <c r="G128" s="10"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A129" s="15"/>
-      <c r="B129" s="15"/>
-      <c r="C129" s="15"/>
-      <c r="D129" s="15"/>
-      <c r="E129" s="15"/>
-      <c r="F129" s="21"/>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="17"/>
+      <c r="B129" s="17"/>
+      <c r="C129" s="17"/>
+      <c r="D129" s="17"/>
+      <c r="E129" s="17"/>
+      <c r="F129" s="20"/>
       <c r="G129" s="10"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A130" s="15"/>
-      <c r="B130" s="15"/>
-      <c r="C130" s="15"/>
-      <c r="D130" s="15"/>
-      <c r="E130" s="15"/>
-      <c r="F130" s="21"/>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="17"/>
+      <c r="B130" s="17"/>
+      <c r="C130" s="17"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="17"/>
+      <c r="F130" s="20"/>
       <c r="G130" s="10"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A131" s="15"/>
-      <c r="B131" s="15"/>
-      <c r="C131" s="15"/>
-      <c r="D131" s="15"/>
-      <c r="E131" s="15"/>
-      <c r="F131" s="21"/>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="17"/>
+      <c r="B131" s="17"/>
+      <c r="C131" s="17"/>
+      <c r="D131" s="17"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="20"/>
       <c r="G131" s="10"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A132" s="15"/>
-      <c r="B132" s="15"/>
-      <c r="C132" s="15"/>
-      <c r="D132" s="15"/>
-      <c r="E132" s="15"/>
-      <c r="F132" s="21"/>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="17"/>
+      <c r="B132" s="17"/>
+      <c r="C132" s="17"/>
+      <c r="D132" s="17"/>
+      <c r="E132" s="17"/>
+      <c r="F132" s="20"/>
       <c r="G132" s="10"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A133" s="16"/>
-      <c r="B133" s="15"/>
-      <c r="C133" s="16"/>
-      <c r="D133" s="16"/>
-      <c r="E133" s="16"/>
-      <c r="F133" s="22"/>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="18"/>
+      <c r="B133" s="17"/>
+      <c r="C133" s="18"/>
+      <c r="D133" s="18"/>
+      <c r="E133" s="18"/>
+      <c r="F133" s="21"/>
       <c r="G133" s="10"/>
     </row>
-    <row r="134" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="14">
+    <row r="134" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="16">
         <v>2.8</v>
       </c>
-      <c r="B134" s="15"/>
-      <c r="C134" s="14" t="s">
+      <c r="B134" s="17"/>
+      <c r="C134" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D134" s="14"/>
-      <c r="E134" s="14" t="s">
+      <c r="D134" s="16"/>
+      <c r="E134" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F134" s="20" t="s">
+      <c r="F134" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G134" s="10"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A135" s="15"/>
-      <c r="B135" s="15"/>
-      <c r="C135" s="15"/>
-      <c r="D135" s="15"/>
-      <c r="E135" s="15"/>
-      <c r="F135" s="21"/>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="17"/>
+      <c r="B135" s="17"/>
+      <c r="C135" s="17"/>
+      <c r="D135" s="17"/>
+      <c r="E135" s="17"/>
+      <c r="F135" s="20"/>
       <c r="G135" s="10"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A136" s="15"/>
-      <c r="B136" s="15"/>
-      <c r="C136" s="15"/>
-      <c r="D136" s="15"/>
-      <c r="E136" s="15"/>
-      <c r="F136" s="21"/>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="17"/>
+      <c r="B136" s="17"/>
+      <c r="C136" s="17"/>
+      <c r="D136" s="17"/>
+      <c r="E136" s="17"/>
+      <c r="F136" s="20"/>
       <c r="G136" s="10"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A137" s="15"/>
-      <c r="B137" s="15"/>
-      <c r="C137" s="15"/>
-      <c r="D137" s="15"/>
-      <c r="E137" s="15"/>
-      <c r="F137" s="21"/>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="17"/>
+      <c r="B137" s="17"/>
+      <c r="C137" s="17"/>
+      <c r="D137" s="17"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="20"/>
       <c r="G137" s="10"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A138" s="15"/>
-      <c r="B138" s="15"/>
-      <c r="C138" s="15"/>
-      <c r="D138" s="15"/>
-      <c r="E138" s="15"/>
-      <c r="F138" s="21"/>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="17"/>
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="20"/>
       <c r="G138" s="10"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A139" s="15"/>
-      <c r="B139" s="15"/>
-      <c r="C139" s="15"/>
-      <c r="D139" s="15"/>
-      <c r="E139" s="15"/>
-      <c r="F139" s="21"/>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="17"/>
+      <c r="B139" s="17"/>
+      <c r="C139" s="17"/>
+      <c r="D139" s="17"/>
+      <c r="E139" s="17"/>
+      <c r="F139" s="20"/>
       <c r="G139" s="10"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A140" s="15"/>
-      <c r="B140" s="15"/>
-      <c r="C140" s="15"/>
-      <c r="D140" s="15"/>
-      <c r="E140" s="15"/>
-      <c r="F140" s="21"/>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="17"/>
+      <c r="B140" s="17"/>
+      <c r="C140" s="17"/>
+      <c r="D140" s="17"/>
+      <c r="E140" s="17"/>
+      <c r="F140" s="20"/>
       <c r="G140" s="10"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A141" s="15"/>
-      <c r="B141" s="15"/>
-      <c r="C141" s="15"/>
-      <c r="D141" s="15"/>
-      <c r="E141" s="15"/>
-      <c r="F141" s="21"/>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="17"/>
+      <c r="B141" s="17"/>
+      <c r="C141" s="17"/>
+      <c r="D141" s="17"/>
+      <c r="E141" s="17"/>
+      <c r="F141" s="20"/>
       <c r="G141" s="10"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A142" s="15"/>
-      <c r="B142" s="15"/>
-      <c r="C142" s="15"/>
-      <c r="D142" s="15"/>
-      <c r="E142" s="15"/>
-      <c r="F142" s="21"/>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="17"/>
+      <c r="B142" s="17"/>
+      <c r="C142" s="17"/>
+      <c r="D142" s="17"/>
+      <c r="E142" s="17"/>
+      <c r="F142" s="20"/>
       <c r="G142" s="10"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A143" s="15"/>
-      <c r="B143" s="15"/>
-      <c r="C143" s="15"/>
-      <c r="D143" s="15"/>
-      <c r="E143" s="15"/>
-      <c r="F143" s="21"/>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="17"/>
+      <c r="B143" s="17"/>
+      <c r="C143" s="17"/>
+      <c r="D143" s="17"/>
+      <c r="E143" s="17"/>
+      <c r="F143" s="20"/>
       <c r="G143" s="10"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A144" s="16"/>
-      <c r="B144" s="15"/>
-      <c r="C144" s="16"/>
-      <c r="D144" s="16"/>
-      <c r="E144" s="16"/>
-      <c r="F144" s="22"/>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="18"/>
+      <c r="B144" s="17"/>
+      <c r="C144" s="18"/>
+      <c r="D144" s="18"/>
+      <c r="E144" s="18"/>
+      <c r="F144" s="21"/>
       <c r="G144" s="10"/>
     </row>
-    <row r="145" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="10">
         <v>2.9</v>
       </c>
-      <c r="B145" s="15"/>
+      <c r="B145" s="17"/>
       <c r="C145" s="10" t="s">
         <v>60</v>
       </c>
@@ -3665,11 +3682,11 @@
       </c>
       <c r="G145" s="10"/>
     </row>
-    <row r="146" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B146" s="15"/>
+      <c r="B146" s="17"/>
       <c r="C146" s="10" t="s">
         <v>61</v>
       </c>
@@ -3682,109 +3699,109 @@
       </c>
       <c r="G146" s="10"/>
     </row>
-    <row r="147" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="14" t="s">
+    <row r="147" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B147" s="15"/>
-      <c r="C147" s="14" t="s">
+      <c r="B147" s="17"/>
+      <c r="C147" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D147" s="14"/>
-      <c r="E147" s="14" t="s">
+      <c r="D147" s="16"/>
+      <c r="E147" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F147" s="17" t="s">
+      <c r="F147" s="25" t="s">
         <v>16</v>
       </c>
       <c r="G147" s="10"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A148" s="15"/>
-      <c r="B148" s="15"/>
-      <c r="C148" s="15"/>
-      <c r="D148" s="15"/>
-      <c r="E148" s="15"/>
-      <c r="F148" s="18"/>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="17"/>
+      <c r="B148" s="17"/>
+      <c r="C148" s="17"/>
+      <c r="D148" s="17"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="26"/>
       <c r="G148" s="10"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A149" s="15"/>
-      <c r="B149" s="15"/>
-      <c r="C149" s="15"/>
-      <c r="D149" s="15"/>
-      <c r="E149" s="15"/>
-      <c r="F149" s="18"/>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="17"/>
+      <c r="B149" s="17"/>
+      <c r="C149" s="17"/>
+      <c r="D149" s="17"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="26"/>
       <c r="G149" s="10"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A150" s="15"/>
-      <c r="B150" s="15"/>
-      <c r="C150" s="15"/>
-      <c r="D150" s="15"/>
-      <c r="E150" s="15"/>
-      <c r="F150" s="18"/>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="17"/>
+      <c r="B150" s="17"/>
+      <c r="C150" s="17"/>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="26"/>
       <c r="G150" s="10"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A151" s="15"/>
-      <c r="B151" s="15"/>
-      <c r="C151" s="15"/>
-      <c r="D151" s="15"/>
-      <c r="E151" s="15"/>
-      <c r="F151" s="18"/>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="17"/>
+      <c r="B151" s="17"/>
+      <c r="C151" s="17"/>
+      <c r="D151" s="17"/>
+      <c r="E151" s="17"/>
+      <c r="F151" s="26"/>
       <c r="G151" s="10"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A152" s="15"/>
-      <c r="B152" s="15"/>
-      <c r="C152" s="15"/>
-      <c r="D152" s="15"/>
-      <c r="E152" s="15"/>
-      <c r="F152" s="18"/>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="17"/>
+      <c r="B152" s="17"/>
+      <c r="C152" s="17"/>
+      <c r="D152" s="17"/>
+      <c r="E152" s="17"/>
+      <c r="F152" s="26"/>
       <c r="G152" s="10"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A153" s="15"/>
-      <c r="B153" s="15"/>
-      <c r="C153" s="15"/>
-      <c r="D153" s="15"/>
-      <c r="E153" s="15"/>
-      <c r="F153" s="18"/>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="17"/>
+      <c r="B153" s="17"/>
+      <c r="C153" s="17"/>
+      <c r="D153" s="17"/>
+      <c r="E153" s="17"/>
+      <c r="F153" s="26"/>
       <c r="G153" s="10"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A154" s="15"/>
-      <c r="B154" s="15"/>
-      <c r="C154" s="15"/>
-      <c r="D154" s="15"/>
-      <c r="E154" s="15"/>
-      <c r="F154" s="18"/>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="17"/>
+      <c r="B154" s="17"/>
+      <c r="C154" s="17"/>
+      <c r="D154" s="17"/>
+      <c r="E154" s="17"/>
+      <c r="F154" s="26"/>
       <c r="G154" s="10"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A155" s="15"/>
-      <c r="B155" s="15"/>
-      <c r="C155" s="15"/>
-      <c r="D155" s="15"/>
-      <c r="E155" s="15"/>
-      <c r="F155" s="18"/>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="17"/>
+      <c r="B155" s="17"/>
+      <c r="C155" s="17"/>
+      <c r="D155" s="17"/>
+      <c r="E155" s="17"/>
+      <c r="F155" s="26"/>
       <c r="G155" s="10"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A156" s="16"/>
-      <c r="B156" s="15"/>
-      <c r="C156" s="16"/>
-      <c r="D156" s="16"/>
-      <c r="E156" s="16"/>
-      <c r="F156" s="19"/>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="18"/>
+      <c r="B156" s="17"/>
+      <c r="C156" s="18"/>
+      <c r="D156" s="18"/>
+      <c r="E156" s="18"/>
+      <c r="F156" s="27"/>
       <c r="G156" s="10"/>
     </row>
-    <row r="157" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B157" s="15"/>
+      <c r="B157" s="17"/>
       <c r="C157" s="10" t="s">
         <v>69</v>
       </c>
@@ -3797,107 +3814,107 @@
       </c>
       <c r="G157" s="10"/>
     </row>
-    <row r="158" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="B158" s="15"/>
+        <v>177</v>
+      </c>
+      <c r="B158" s="17"/>
       <c r="C158" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D158" s="10"/>
       <c r="E158" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F158" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G158" s="10"/>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A159" s="14" t="s">
+    <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B159" s="17"/>
+      <c r="C159" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="B159" s="15"/>
-      <c r="C159" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="D159" s="10"/>
       <c r="E159" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F159" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G159" s="10"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A160" s="15"/>
-      <c r="B160" s="15"/>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="17"/>
+      <c r="B160" s="17"/>
       <c r="C160" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D160" s="10"/>
       <c r="E160" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F160" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G160" s="10"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A161" s="16"/>
-      <c r="B161" s="16"/>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="18"/>
+      <c r="B161" s="18"/>
       <c r="C161" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D161" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E161" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F161" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G161" s="10"/>
     </row>
-    <row r="162" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B162" s="11"/>
       <c r="C162" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D162" s="10"/>
       <c r="E162" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F162" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G162" s="10"/>
     </row>
-    <row r="163" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="11">
         <v>2.16</v>
       </c>
       <c r="B163" s="11"/>
       <c r="C163" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D163" s="10"/>
       <c r="E163" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F163" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G163" s="10"/>
     </row>
-    <row r="164" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="9">
         <v>3</v>
       </c>
@@ -3910,116 +3927,116 @@
       <c r="F164" s="9"/>
       <c r="G164" s="9"/>
     </row>
-    <row r="165" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="14">
+    <row r="165" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="16">
         <v>3.1</v>
       </c>
-      <c r="B165" s="14" t="s">
+      <c r="B165" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C165" s="14" t="s">
+      <c r="C165" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="D165" s="14"/>
-      <c r="E165" s="14" t="s">
+      <c r="D165" s="16"/>
+      <c r="E165" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F165" s="17" t="s">
-        <v>16</v>
+      <c r="F165" s="28" t="s">
+        <v>10</v>
       </c>
       <c r="G165" s="10"/>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A166" s="15"/>
-      <c r="B166" s="15"/>
-      <c r="C166" s="15"/>
-      <c r="D166" s="15"/>
-      <c r="E166" s="15"/>
-      <c r="F166" s="18"/>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="17"/>
+      <c r="B166" s="17"/>
+      <c r="C166" s="17"/>
+      <c r="D166" s="17"/>
+      <c r="E166" s="17"/>
+      <c r="F166" s="29"/>
       <c r="G166" s="10"/>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A167" s="15"/>
-      <c r="B167" s="15"/>
-      <c r="C167" s="15"/>
-      <c r="D167" s="15"/>
-      <c r="E167" s="15"/>
-      <c r="F167" s="18"/>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="17"/>
+      <c r="B167" s="17"/>
+      <c r="C167" s="17"/>
+      <c r="D167" s="17"/>
+      <c r="E167" s="17"/>
+      <c r="F167" s="29"/>
       <c r="G167" s="10"/>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A168" s="15"/>
-      <c r="B168" s="15"/>
-      <c r="C168" s="15"/>
-      <c r="D168" s="15"/>
-      <c r="E168" s="15"/>
-      <c r="F168" s="18"/>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" s="17"/>
+      <c r="B168" s="17"/>
+      <c r="C168" s="17"/>
+      <c r="D168" s="17"/>
+      <c r="E168" s="17"/>
+      <c r="F168" s="29"/>
       <c r="G168" s="10"/>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A169" s="15"/>
-      <c r="B169" s="15"/>
-      <c r="C169" s="15"/>
-      <c r="D169" s="15"/>
-      <c r="E169" s="15"/>
-      <c r="F169" s="18"/>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="17"/>
+      <c r="B169" s="17"/>
+      <c r="C169" s="17"/>
+      <c r="D169" s="17"/>
+      <c r="E169" s="17"/>
+      <c r="F169" s="29"/>
       <c r="G169" s="10"/>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A170" s="15"/>
-      <c r="B170" s="15"/>
-      <c r="C170" s="15"/>
-      <c r="D170" s="15"/>
-      <c r="E170" s="15"/>
-      <c r="F170" s="18"/>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="17"/>
+      <c r="B170" s="17"/>
+      <c r="C170" s="17"/>
+      <c r="D170" s="17"/>
+      <c r="E170" s="17"/>
+      <c r="F170" s="29"/>
       <c r="G170" s="10"/>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A171" s="15"/>
-      <c r="B171" s="15"/>
-      <c r="C171" s="15"/>
-      <c r="D171" s="15"/>
-      <c r="E171" s="15"/>
-      <c r="F171" s="18"/>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="17"/>
+      <c r="B171" s="17"/>
+      <c r="C171" s="17"/>
+      <c r="D171" s="17"/>
+      <c r="E171" s="17"/>
+      <c r="F171" s="29"/>
       <c r="G171" s="10"/>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A172" s="15"/>
-      <c r="B172" s="15"/>
-      <c r="C172" s="15"/>
-      <c r="D172" s="15"/>
-      <c r="E172" s="15"/>
-      <c r="F172" s="18"/>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="17"/>
+      <c r="B172" s="17"/>
+      <c r="C172" s="17"/>
+      <c r="D172" s="17"/>
+      <c r="E172" s="17"/>
+      <c r="F172" s="29"/>
       <c r="G172" s="10"/>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A173" s="15"/>
-      <c r="B173" s="15"/>
-      <c r="C173" s="15"/>
-      <c r="D173" s="15"/>
-      <c r="E173" s="15"/>
-      <c r="F173" s="18"/>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="17"/>
+      <c r="B173" s="17"/>
+      <c r="C173" s="17"/>
+      <c r="D173" s="17"/>
+      <c r="E173" s="17"/>
+      <c r="F173" s="29"/>
       <c r="G173" s="10"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A174" s="16"/>
-      <c r="B174" s="15"/>
-      <c r="C174" s="16"/>
-      <c r="D174" s="16"/>
-      <c r="E174" s="16"/>
-      <c r="F174" s="19"/>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="18"/>
+      <c r="B174" s="17"/>
+      <c r="C174" s="18"/>
+      <c r="D174" s="18"/>
+      <c r="E174" s="18"/>
+      <c r="F174" s="30"/>
       <c r="G174" s="10"/>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="10">
         <v>3.2</v>
       </c>
-      <c r="B175" s="15"/>
+      <c r="B175" s="17"/>
       <c r="C175" s="10" t="s">
         <v>72</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E175" s="10" t="s">
         <v>73</v>
@@ -4029,16 +4046,16 @@
       </c>
       <c r="G175" s="10"/>
     </row>
-    <row r="176" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="10">
         <v>3.3</v>
       </c>
-      <c r="B176" s="15"/>
+      <c r="B176" s="17"/>
       <c r="C176" s="10" t="s">
         <v>74</v>
       </c>
       <c r="D176" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E176" s="10" t="s">
         <v>75</v>
@@ -4048,173 +4065,173 @@
       </c>
       <c r="G176" s="10"/>
     </row>
-    <row r="177" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="10">
         <v>3.4</v>
       </c>
-      <c r="B177" s="15"/>
+      <c r="B177" s="17"/>
       <c r="C177" s="10" t="s">
         <v>76</v>
       </c>
       <c r="D177" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E177" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F177" s="12" t="s">
+      <c r="F177" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G177" s="10"/>
+    </row>
+    <row r="178" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="B178" s="17"/>
+      <c r="C178" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="G177" s="10"/>
-    </row>
-    <row r="178" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="14">
-        <v>3.5</v>
-      </c>
-      <c r="B178" s="15"/>
-      <c r="C178" s="14" t="s">
+      <c r="D178" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D178" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E178" s="14" t="s">
+      <c r="E178" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F178" s="17" t="s">
-        <v>16</v>
+      <c r="F178" s="28" t="s">
+        <v>10</v>
       </c>
       <c r="G178" s="10"/>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A179" s="15"/>
-      <c r="B179" s="15"/>
-      <c r="C179" s="15"/>
-      <c r="D179" s="15"/>
-      <c r="E179" s="15"/>
-      <c r="F179" s="18"/>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="17"/>
+      <c r="B179" s="17"/>
+      <c r="C179" s="17"/>
+      <c r="D179" s="17"/>
+      <c r="E179" s="17"/>
+      <c r="F179" s="29"/>
       <c r="G179" s="10"/>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A180" s="15"/>
-      <c r="B180" s="15"/>
-      <c r="C180" s="15"/>
-      <c r="D180" s="15"/>
-      <c r="E180" s="15"/>
-      <c r="F180" s="18"/>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="17"/>
+      <c r="B180" s="17"/>
+      <c r="C180" s="17"/>
+      <c r="D180" s="17"/>
+      <c r="E180" s="17"/>
+      <c r="F180" s="29"/>
       <c r="G180" s="10"/>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A181" s="15"/>
-      <c r="B181" s="15"/>
-      <c r="C181" s="15"/>
-      <c r="D181" s="15"/>
-      <c r="E181" s="15"/>
-      <c r="F181" s="18"/>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="17"/>
+      <c r="B181" s="17"/>
+      <c r="C181" s="17"/>
+      <c r="D181" s="17"/>
+      <c r="E181" s="17"/>
+      <c r="F181" s="29"/>
       <c r="G181" s="10"/>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A182" s="15"/>
-      <c r="B182" s="15"/>
-      <c r="C182" s="15"/>
-      <c r="D182" s="15"/>
-      <c r="E182" s="15"/>
-      <c r="F182" s="18"/>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="17"/>
+      <c r="B182" s="17"/>
+      <c r="C182" s="17"/>
+      <c r="D182" s="17"/>
+      <c r="E182" s="17"/>
+      <c r="F182" s="29"/>
       <c r="G182" s="10"/>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A183" s="15"/>
-      <c r="B183" s="15"/>
-      <c r="C183" s="15"/>
-      <c r="D183" s="15"/>
-      <c r="E183" s="15"/>
-      <c r="F183" s="18"/>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="17"/>
+      <c r="B183" s="17"/>
+      <c r="C183" s="17"/>
+      <c r="D183" s="17"/>
+      <c r="E183" s="17"/>
+      <c r="F183" s="29"/>
       <c r="G183" s="10"/>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A184" s="15"/>
-      <c r="B184" s="15"/>
-      <c r="C184" s="15"/>
-      <c r="D184" s="15"/>
-      <c r="E184" s="15"/>
-      <c r="F184" s="18"/>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="17"/>
+      <c r="B184" s="17"/>
+      <c r="C184" s="17"/>
+      <c r="D184" s="17"/>
+      <c r="E184" s="17"/>
+      <c r="F184" s="29"/>
       <c r="G184" s="10"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A185" s="15"/>
-      <c r="B185" s="15"/>
-      <c r="C185" s="15"/>
-      <c r="D185" s="15"/>
-      <c r="E185" s="15"/>
-      <c r="F185" s="18"/>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="17"/>
+      <c r="B185" s="17"/>
+      <c r="C185" s="17"/>
+      <c r="D185" s="17"/>
+      <c r="E185" s="17"/>
+      <c r="F185" s="29"/>
       <c r="G185" s="10"/>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A186" s="15"/>
-      <c r="B186" s="15"/>
-      <c r="C186" s="15"/>
-      <c r="D186" s="15"/>
-      <c r="E186" s="15"/>
-      <c r="F186" s="18"/>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="17"/>
+      <c r="B186" s="17"/>
+      <c r="C186" s="17"/>
+      <c r="D186" s="17"/>
+      <c r="E186" s="17"/>
+      <c r="F186" s="29"/>
       <c r="G186" s="10"/>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A187" s="16"/>
-      <c r="B187" s="15"/>
-      <c r="C187" s="16"/>
-      <c r="D187" s="16"/>
-      <c r="E187" s="16"/>
-      <c r="F187" s="19"/>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="18"/>
+      <c r="B187" s="17"/>
+      <c r="C187" s="18"/>
+      <c r="D187" s="18"/>
+      <c r="E187" s="18"/>
+      <c r="F187" s="30"/>
       <c r="G187" s="10"/>
     </row>
-    <row r="188" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="10">
         <v>3.6</v>
       </c>
-      <c r="B188" s="15"/>
+      <c r="B188" s="17"/>
       <c r="C188" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E188" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F188" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G188" s="10"/>
     </row>
-    <row r="189" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="10">
         <v>3.7</v>
       </c>
-      <c r="B189" s="15"/>
+      <c r="B189" s="17"/>
       <c r="C189" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E189" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F189" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G189" s="10"/>
     </row>
-    <row r="190" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="10">
         <v>3.8</v>
       </c>
-      <c r="B190" s="15"/>
+      <c r="B190" s="17"/>
       <c r="C190" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E190" s="10" t="s">
         <v>75</v>
@@ -4224,547 +4241,547 @@
       </c>
       <c r="G190" s="10"/>
     </row>
-    <row r="191" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="14">
+    <row r="191" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="16">
         <v>3.9</v>
       </c>
-      <c r="B191" s="15"/>
-      <c r="C191" s="14" t="s">
+      <c r="B191" s="17"/>
+      <c r="C191" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D191" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D191" s="14" t="s">
+      <c r="E191" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F191" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G191" s="10"/>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="17"/>
+      <c r="B192" s="17"/>
+      <c r="C192" s="17"/>
+      <c r="D192" s="17"/>
+      <c r="E192" s="17"/>
+      <c r="F192" s="29"/>
+      <c r="G192" s="10"/>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193" s="17"/>
+      <c r="B193" s="17"/>
+      <c r="C193" s="17"/>
+      <c r="D193" s="17"/>
+      <c r="E193" s="17"/>
+      <c r="F193" s="29"/>
+      <c r="G193" s="10"/>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" s="17"/>
+      <c r="B194" s="17"/>
+      <c r="C194" s="17"/>
+      <c r="D194" s="17"/>
+      <c r="E194" s="17"/>
+      <c r="F194" s="29"/>
+      <c r="G194" s="10"/>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195" s="17"/>
+      <c r="B195" s="17"/>
+      <c r="C195" s="17"/>
+      <c r="D195" s="17"/>
+      <c r="E195" s="17"/>
+      <c r="F195" s="29"/>
+      <c r="G195" s="10"/>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A196" s="17"/>
+      <c r="B196" s="17"/>
+      <c r="C196" s="17"/>
+      <c r="D196" s="17"/>
+      <c r="E196" s="17"/>
+      <c r="F196" s="29"/>
+      <c r="G196" s="10"/>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A197" s="17"/>
+      <c r="B197" s="17"/>
+      <c r="C197" s="17"/>
+      <c r="D197" s="17"/>
+      <c r="E197" s="17"/>
+      <c r="F197" s="29"/>
+      <c r="G197" s="10"/>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198" s="17"/>
+      <c r="B198" s="17"/>
+      <c r="C198" s="17"/>
+      <c r="D198" s="17"/>
+      <c r="E198" s="17"/>
+      <c r="F198" s="29"/>
+      <c r="G198" s="10"/>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A199" s="17"/>
+      <c r="B199" s="17"/>
+      <c r="C199" s="17"/>
+      <c r="D199" s="17"/>
+      <c r="E199" s="17"/>
+      <c r="F199" s="29"/>
+      <c r="G199" s="10"/>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A200" s="18"/>
+      <c r="B200" s="17"/>
+      <c r="C200" s="18"/>
+      <c r="D200" s="18"/>
+      <c r="E200" s="18"/>
+      <c r="F200" s="30"/>
+      <c r="G200" s="10"/>
+    </row>
+    <row r="201" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B201" s="17"/>
+      <c r="C201" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D201" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E191" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F191" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G191" s="10"/>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A192" s="15"/>
-      <c r="B192" s="15"/>
-      <c r="C192" s="15"/>
-      <c r="D192" s="15"/>
-      <c r="E192" s="15"/>
-      <c r="F192" s="18"/>
-      <c r="G192" s="10"/>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A193" s="15"/>
-      <c r="B193" s="15"/>
-      <c r="C193" s="15"/>
-      <c r="D193" s="15"/>
-      <c r="E193" s="15"/>
-      <c r="F193" s="18"/>
-      <c r="G193" s="10"/>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A194" s="15"/>
-      <c r="B194" s="15"/>
-      <c r="C194" s="15"/>
-      <c r="D194" s="15"/>
-      <c r="E194" s="15"/>
-      <c r="F194" s="18"/>
-      <c r="G194" s="10"/>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A195" s="15"/>
-      <c r="B195" s="15"/>
-      <c r="C195" s="15"/>
-      <c r="D195" s="15"/>
-      <c r="E195" s="15"/>
-      <c r="F195" s="18"/>
-      <c r="G195" s="10"/>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A196" s="15"/>
-      <c r="B196" s="15"/>
-      <c r="C196" s="15"/>
-      <c r="D196" s="15"/>
-      <c r="E196" s="15"/>
-      <c r="F196" s="18"/>
-      <c r="G196" s="10"/>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A197" s="15"/>
-      <c r="B197" s="15"/>
-      <c r="C197" s="15"/>
-      <c r="D197" s="15"/>
-      <c r="E197" s="15"/>
-      <c r="F197" s="18"/>
-      <c r="G197" s="10"/>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A198" s="15"/>
-      <c r="B198" s="15"/>
-      <c r="C198" s="15"/>
-      <c r="D198" s="15"/>
-      <c r="E198" s="15"/>
-      <c r="F198" s="18"/>
-      <c r="G198" s="10"/>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A199" s="15"/>
-      <c r="B199" s="15"/>
-      <c r="C199" s="15"/>
-      <c r="D199" s="15"/>
-      <c r="E199" s="15"/>
-      <c r="F199" s="18"/>
-      <c r="G199" s="10"/>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A200" s="16"/>
-      <c r="B200" s="15"/>
-      <c r="C200" s="16"/>
-      <c r="D200" s="16"/>
-      <c r="E200" s="16"/>
-      <c r="F200" s="19"/>
-      <c r="G200" s="10"/>
-    </row>
-    <row r="201" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A201" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B201" s="15"/>
-      <c r="C201" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D201" s="10" t="s">
+      <c r="E201" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E201" s="10" t="s">
-        <v>86</v>
-      </c>
       <c r="F201" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G201" s="10"/>
     </row>
-    <row r="202" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="10">
         <v>3.11</v>
       </c>
-      <c r="B202" s="15"/>
+      <c r="B202" s="17"/>
       <c r="C202" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D202" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E202" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F202" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F202" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G202" s="10"/>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="10">
         <v>3.12</v>
       </c>
-      <c r="B203" s="15"/>
+      <c r="B203" s="17"/>
       <c r="C203" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D203" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="D203" s="10" t="s">
-        <v>96</v>
       </c>
       <c r="E203" s="10"/>
       <c r="F203" s="10"/>
       <c r="G203" s="10"/>
     </row>
-    <row r="204" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="10">
         <v>3.13</v>
       </c>
-      <c r="B204" s="15"/>
+      <c r="B204" s="17"/>
       <c r="C204" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D204" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D204" s="10" t="s">
+      <c r="E204" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E204" s="10" t="s">
-        <v>100</v>
-      </c>
       <c r="F204" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G204" s="10"/>
     </row>
-    <row r="205" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="10">
         <v>3.14</v>
       </c>
-      <c r="B205" s="15"/>
+      <c r="B205" s="17"/>
       <c r="C205" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D205" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D205" s="10" t="s">
-        <v>117</v>
-      </c>
       <c r="E205" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F205" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G205" s="10"/>
     </row>
-    <row r="206" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="10">
         <v>3.15</v>
       </c>
-      <c r="B206" s="15"/>
+      <c r="B206" s="17"/>
       <c r="C206" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D206" s="10"/>
       <c r="E206" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F206" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G206" s="10"/>
     </row>
-    <row r="207" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A207" s="10">
         <v>3.16</v>
       </c>
-      <c r="B207" s="15"/>
+      <c r="B207" s="17"/>
       <c r="C207" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D207" s="10"/>
       <c r="E207" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F207" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G207" s="10"/>
     </row>
-    <row r="208" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A208" s="10">
         <v>3.17</v>
       </c>
-      <c r="B208" s="15"/>
+      <c r="B208" s="17"/>
       <c r="C208" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D208" s="10"/>
       <c r="E208" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F208" s="12" t="s">
         <v>122</v>
       </c>
+      <c r="F208" s="31" t="s">
+        <v>10</v>
+      </c>
       <c r="G208" s="10"/>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="10">
         <v>3.18</v>
       </c>
-      <c r="B209" s="15"/>
+      <c r="B209" s="17"/>
       <c r="C209" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D209" s="10"/>
       <c r="E209" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F209" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G209" s="10"/>
     </row>
-    <row r="210" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="10">
         <v>3.19</v>
       </c>
-      <c r="B210" s="15"/>
+      <c r="B210" s="17"/>
       <c r="C210" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D210" s="10"/>
       <c r="E210" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F210" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G210" s="10"/>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B211" s="15"/>
+        <v>130</v>
+      </c>
+      <c r="B211" s="17"/>
       <c r="C211" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D211" s="10"/>
       <c r="E211" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F211" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G211" s="10"/>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="10">
         <v>3.21</v>
       </c>
-      <c r="B212" s="15"/>
+      <c r="B212" s="17"/>
       <c r="C212" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D212" s="10"/>
       <c r="E212" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F212" s="12" t="s">
-        <v>122</v>
+        <v>129</v>
+      </c>
+      <c r="F212" s="31" t="s">
+        <v>10</v>
       </c>
       <c r="G212" s="10"/>
     </row>
-    <row r="213" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="10">
         <v>3.22</v>
       </c>
-      <c r="B213" s="15"/>
+      <c r="B213" s="17"/>
       <c r="C213" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D213" s="10"/>
       <c r="E213" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F213" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G213" s="10"/>
     </row>
-    <row r="214" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="10">
         <v>3.23</v>
       </c>
-      <c r="B214" s="15"/>
+      <c r="B214" s="17"/>
       <c r="C214" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D214" s="10"/>
       <c r="E214" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F214" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G214" s="10"/>
     </row>
-    <row r="215" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A215" s="10">
         <v>3.24</v>
       </c>
-      <c r="B215" s="15"/>
+      <c r="B215" s="17"/>
       <c r="C215" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D215" s="10"/>
       <c r="E215" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F215" s="12" t="s">
-        <v>140</v>
+        <v>137</v>
+      </c>
+      <c r="F215" s="31" t="s">
+        <v>10</v>
       </c>
       <c r="G215" s="10"/>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="10">
         <v>3.25</v>
       </c>
-      <c r="B216" s="15"/>
+      <c r="B216" s="17"/>
       <c r="C216" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D216" s="10"/>
       <c r="E216" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F216" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G216" s="10"/>
     </row>
-    <row r="217" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="10">
         <v>3.26</v>
       </c>
-      <c r="B217" s="15"/>
+      <c r="B217" s="17"/>
       <c r="C217" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D217" s="10"/>
       <c r="E217" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F217" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G217" s="10"/>
     </row>
-    <row r="218" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A218" s="10">
         <v>3.27</v>
       </c>
-      <c r="B218" s="15"/>
+      <c r="B218" s="17"/>
       <c r="C218" s="10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D218" s="10"/>
       <c r="E218" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="F218" s="12" t="s">
-        <v>122</v>
+        <v>143</v>
+      </c>
+      <c r="F218" s="31" t="s">
+        <v>10</v>
       </c>
       <c r="G218" s="10"/>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="10">
         <v>3.28</v>
       </c>
-      <c r="B219" s="15"/>
+      <c r="B219" s="17"/>
       <c r="C219" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D219" s="10"/>
       <c r="E219" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F219" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G219" s="10"/>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="10">
         <v>3.29</v>
       </c>
-      <c r="B220" s="15"/>
+      <c r="B220" s="17"/>
       <c r="C220" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D220" s="10"/>
       <c r="E220" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F220" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G220" s="10"/>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A221" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F220" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G220" s="10"/>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A221" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="B221" s="15"/>
+      <c r="B221" s="17"/>
       <c r="C221" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D221" s="10"/>
       <c r="E221" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F221" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G221" s="10"/>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="10">
         <v>3.31</v>
       </c>
-      <c r="B222" s="15"/>
+      <c r="B222" s="17"/>
       <c r="C222" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D222" s="10"/>
       <c r="E222" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F222" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G222" s="10"/>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="10">
         <v>3.32</v>
       </c>
-      <c r="B223" s="15"/>
+      <c r="B223" s="17"/>
       <c r="C223" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D223" s="10"/>
       <c r="E223" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F223" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G223" s="10"/>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="10">
         <v>3.33</v>
       </c>
-      <c r="B224" s="15"/>
+      <c r="B224" s="17"/>
       <c r="C224" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D224" s="10"/>
       <c r="E224" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F224" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G224" s="10"/>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="10">
         <v>3.34</v>
       </c>
-      <c r="B225" s="15"/>
+      <c r="B225" s="17"/>
       <c r="C225" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D225" s="10"/>
       <c r="E225" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F225" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G225" s="10"/>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="10">
         <v>3.35</v>
       </c>
-      <c r="B226" s="15"/>
+      <c r="B226" s="17"/>
       <c r="C226" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D226" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E226" s="10" t="s">
         <v>56</v>
@@ -4774,16 +4791,16 @@
       </c>
       <c r="G226" s="10"/>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="10">
         <v>3.36</v>
       </c>
-      <c r="B227" s="16"/>
+      <c r="B227" s="18"/>
       <c r="C227" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D227" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E227" s="10" t="s">
         <v>56</v>
@@ -4793,12 +4810,12 @@
       </c>
       <c r="G227" s="10"/>
     </row>
-    <row r="228" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="9">
         <v>4</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C228" s="9"/>
       <c r="D228" s="9"/>
@@ -4806,209 +4823,209 @@
       <c r="F228" s="9"/>
       <c r="G228" s="9"/>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="10">
         <v>4.0999999999999996</v>
       </c>
       <c r="B229" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C229" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D229" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E229" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="C229" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D229" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="E229" s="10" t="s">
-        <v>163</v>
-      </c>
       <c r="F229" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G229" s="10"/>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="10">
         <v>4.2</v>
       </c>
       <c r="B230" s="10"/>
       <c r="C230" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D230" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E230" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F230" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G230" s="10"/>
     </row>
-    <row r="231" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="10">
         <v>4.3</v>
       </c>
       <c r="B231" s="10"/>
       <c r="C231" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D231" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E231" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="F231" s="12" t="s">
-        <v>16</v>
+        <v>191</v>
+      </c>
+      <c r="F231" s="31" t="s">
+        <v>10</v>
       </c>
       <c r="G231" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="232" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="10">
         <v>4.4000000000000004</v>
       </c>
       <c r="B232" s="10"/>
       <c r="C232" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D232" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E232" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="F232" s="12" t="s">
-        <v>16</v>
+        <v>191</v>
+      </c>
+      <c r="F232" s="31" t="s">
+        <v>10</v>
       </c>
       <c r="G232" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="233" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="10">
         <v>4.5</v>
       </c>
       <c r="B233" s="10"/>
       <c r="C233" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D233" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E233" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F233" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G233" s="10"/>
     </row>
-    <row r="234" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A234" s="10">
         <v>4.5999999999999996</v>
       </c>
       <c r="B234" s="10"/>
       <c r="C234" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D234" s="10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E234" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F234" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G234" s="10"/>
     </row>
-    <row r="235" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="10">
         <v>4.7</v>
       </c>
       <c r="B235" s="10"/>
       <c r="C235" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D235" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E235" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F235" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G235" s="10"/>
     </row>
-    <row r="236" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" s="10">
         <v>4.8</v>
       </c>
       <c r="B236" s="10"/>
       <c r="C236" s="10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D236" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E236" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F236" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G236" s="10"/>
     </row>
-    <row r="237" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" s="10">
         <v>4.9000000000000004</v>
       </c>
       <c r="B237" s="10"/>
       <c r="C237" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D237" s="10"/>
       <c r="E237" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F237" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G237" s="10"/>
     </row>
-    <row r="238" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B238" s="10"/>
       <c r="C238" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D238" s="10"/>
       <c r="E238" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F238" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G238" s="10"/>
     </row>
-    <row r="239" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" s="10">
         <v>4.1100000000000003</v>
       </c>
       <c r="B239" s="10"/>
       <c r="C239" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D239" s="10"/>
       <c r="E239" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F239" s="13" t="s">
         <v>10</v>
@@ -5017,18 +5034,65 @@
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="A165:A174"/>
-    <mergeCell ref="A178:A187"/>
-    <mergeCell ref="A191:A200"/>
-    <mergeCell ref="B165:B227"/>
-    <mergeCell ref="B97:B161"/>
-    <mergeCell ref="A97:A106"/>
-    <mergeCell ref="A113:A122"/>
-    <mergeCell ref="A107:A109"/>
-    <mergeCell ref="A123:A133"/>
-    <mergeCell ref="A134:A144"/>
-    <mergeCell ref="A147:A156"/>
-    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="F113:F122"/>
+    <mergeCell ref="F123:F133"/>
+    <mergeCell ref="F134:F144"/>
+    <mergeCell ref="F147:F156"/>
+    <mergeCell ref="C113:C122"/>
+    <mergeCell ref="C123:C133"/>
+    <mergeCell ref="C134:C144"/>
+    <mergeCell ref="C147:C156"/>
+    <mergeCell ref="E147:E156"/>
+    <mergeCell ref="F191:F200"/>
+    <mergeCell ref="C191:C200"/>
+    <mergeCell ref="D191:D200"/>
+    <mergeCell ref="E191:E200"/>
+    <mergeCell ref="D165:D174"/>
+    <mergeCell ref="F165:F174"/>
+    <mergeCell ref="F178:F187"/>
+    <mergeCell ref="C165:C174"/>
+    <mergeCell ref="E165:E174"/>
+    <mergeCell ref="D178:D187"/>
+    <mergeCell ref="C178:C187"/>
+    <mergeCell ref="E178:E187"/>
+    <mergeCell ref="E123:E133"/>
+    <mergeCell ref="E113:E122"/>
+    <mergeCell ref="D147:D156"/>
+    <mergeCell ref="D134:D144"/>
+    <mergeCell ref="D123:D133"/>
+    <mergeCell ref="D113:D122"/>
+    <mergeCell ref="E134:E144"/>
+    <mergeCell ref="C107:C109"/>
+    <mergeCell ref="C97:C106"/>
+    <mergeCell ref="E97:E106"/>
+    <mergeCell ref="F107:F109"/>
+    <mergeCell ref="F97:F106"/>
+    <mergeCell ref="D97:D106"/>
+    <mergeCell ref="D107:D109"/>
+    <mergeCell ref="F39:F50"/>
+    <mergeCell ref="F51:F60"/>
+    <mergeCell ref="E79:E89"/>
+    <mergeCell ref="F79:F89"/>
+    <mergeCell ref="F68:F78"/>
+    <mergeCell ref="D79:D89"/>
+    <mergeCell ref="D68:D78"/>
+    <mergeCell ref="D51:D60"/>
+    <mergeCell ref="D39:D50"/>
+    <mergeCell ref="E41:E50"/>
+    <mergeCell ref="C11:C19"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="E11:E19"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B3:B89"/>
+    <mergeCell ref="A79:A89"/>
+    <mergeCell ref="D29:D38"/>
+    <mergeCell ref="D20:D28"/>
+    <mergeCell ref="D11:D19"/>
+    <mergeCell ref="D3:D10"/>
+    <mergeCell ref="A29:A38"/>
+    <mergeCell ref="A39:A50"/>
+    <mergeCell ref="C79:C89"/>
     <mergeCell ref="F3:F10"/>
     <mergeCell ref="F11:F19"/>
     <mergeCell ref="F20:F28"/>
@@ -5045,65 +5109,18 @@
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="A11:A19"/>
     <mergeCell ref="C20:C28"/>
-    <mergeCell ref="C11:C19"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="E3:E10"/>
-    <mergeCell ref="E11:E19"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B3:B89"/>
-    <mergeCell ref="A79:A89"/>
-    <mergeCell ref="D29:D38"/>
-    <mergeCell ref="D20:D28"/>
-    <mergeCell ref="D11:D19"/>
-    <mergeCell ref="D3:D10"/>
-    <mergeCell ref="A29:A38"/>
-    <mergeCell ref="A39:A50"/>
-    <mergeCell ref="D97:D106"/>
-    <mergeCell ref="D107:D109"/>
-    <mergeCell ref="F39:F50"/>
-    <mergeCell ref="F51:F60"/>
-    <mergeCell ref="E79:E89"/>
-    <mergeCell ref="F79:F89"/>
-    <mergeCell ref="C79:C89"/>
-    <mergeCell ref="F68:F78"/>
-    <mergeCell ref="D79:D89"/>
-    <mergeCell ref="D68:D78"/>
-    <mergeCell ref="D51:D60"/>
-    <mergeCell ref="D39:D50"/>
-    <mergeCell ref="C107:C109"/>
-    <mergeCell ref="C97:C106"/>
-    <mergeCell ref="E97:E106"/>
-    <mergeCell ref="F107:F109"/>
-    <mergeCell ref="F97:F106"/>
-    <mergeCell ref="E123:E133"/>
-    <mergeCell ref="E113:E122"/>
-    <mergeCell ref="D147:D156"/>
-    <mergeCell ref="D134:D144"/>
-    <mergeCell ref="D123:D133"/>
-    <mergeCell ref="D113:D122"/>
-    <mergeCell ref="E134:E144"/>
-    <mergeCell ref="F165:F174"/>
-    <mergeCell ref="F178:F187"/>
-    <mergeCell ref="C165:C174"/>
-    <mergeCell ref="E165:E174"/>
-    <mergeCell ref="D178:D187"/>
-    <mergeCell ref="C178:C187"/>
-    <mergeCell ref="E178:E187"/>
-    <mergeCell ref="E41:E50"/>
-    <mergeCell ref="F191:F200"/>
-    <mergeCell ref="C191:C200"/>
-    <mergeCell ref="D191:D200"/>
-    <mergeCell ref="E191:E200"/>
-    <mergeCell ref="D165:D174"/>
-    <mergeCell ref="F113:F122"/>
-    <mergeCell ref="F123:F133"/>
-    <mergeCell ref="F134:F144"/>
-    <mergeCell ref="F147:F156"/>
-    <mergeCell ref="C113:C122"/>
-    <mergeCell ref="C123:C133"/>
-    <mergeCell ref="C134:C144"/>
-    <mergeCell ref="C147:C156"/>
-    <mergeCell ref="E147:E156"/>
+    <mergeCell ref="A165:A174"/>
+    <mergeCell ref="A178:A187"/>
+    <mergeCell ref="A191:A200"/>
+    <mergeCell ref="B165:B227"/>
+    <mergeCell ref="B97:B161"/>
+    <mergeCell ref="A97:A106"/>
+    <mergeCell ref="A113:A122"/>
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="A123:A133"/>
+    <mergeCell ref="A134:A144"/>
+    <mergeCell ref="A147:A156"/>
+    <mergeCell ref="A159:A161"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5117,7 +5134,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5129,7 +5146,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>